<commit_message>
update hystreet metadata with info about missing measurements at bahnhofstrasse nord.
</commit_message>
<xml_diff>
--- a/automation/hystreet_fussgaengerfrequenzen/hystreet_fussgaenger_metadata.xlsx
+++ b/automation/hystreet_fussgaengerfrequenzen/hystreet_fussgaenger_metadata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\szh.loc\ssz\users\sszsim\Dokumente\GitHub\opendatazurich\opendatazurich.github.io\automation\hystreet_fussgaengerfrequenzen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\sszsim\opendatazurich\opendatazurich.github.io\automation\hystreet_fussgaengerfrequenzen\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9695273-D77E-4235-9AB2-1652D0551B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="5505"/>
+    <workbookView xWindow="23496" yWindow="456" windowWidth="30960" windowHeight="12156" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -809,11 +810,6 @@
 		</t>
   </si>
   <si>
-    <t>Bei den Zählwerten **vor dem 03.03.2022** (Testbetrieb)  können Inkonsistenzen vorkommen. Ab dem 03.03.2022 ist die Datenqualität in der Regel gut.
-- Bei den Zählungen vor dem 03.03.2022 können Inkonsistenzen auftreten. Im Gebiet «Bahnhofstrasse (Süd)» stimmt bis zum 03.03.2022 die Unterscheidung zwischen Erwachsenen und Kindern nicht. Alle Zählwerte wurden in diesem Zeitraum fäschlicherweise den Kindern zugeordnet.
-- Im Teilgebiet **Bahnhofstrasse (Nord)** fehlen die Messwerte zwischen dem 14.09. – 23.12.2022 wegen Bauarbeiten.</t>
-  </si>
-  <si>
     <t>Die Messung von Passantenfrequenzen kann wichtige Hinweise auf die Attraktivität und die Nutzung von Orten geben. Im Rahmen eines gemeinsamen Pilotprojektes zwischen dem internationalen Immobilienberatungsunternehmen CBRE, dem PropTech Unternehmen hystreet.com, Swiss Life Asset Managers, der Stadtentwicklung Zürich und der Vereinigung Zürcher Bahnhofstrasse werden durch die Firma Hystreet an der Bahnhofstrasse Passantenfrequenzen erhoben. 
 Die Messungen erfolgen mit Laserscannern und werden stündlich aktualisiert. Aktuell gibt es **drei Messgebiete** (siehe [hystreet_locations.json](https://data.stadt-zuerich.ch/dataset/hystreet_fussgaengerfrequenzen/download/hystreet_locations.json)): 
 - Bahnhofstrasse (Nord), 
@@ -835,11 +831,19 @@
 Die Zonen definieren sich über die Strassen- oder Bürgersteigseiten: Die gezählten Passanten sind jeweils einer Bürgersteigseite zugeordnet.
 Bei den Standorten Bahnhofstrase (Nord) und (Süd) ist die Zone 1 die westliche Bürgersteigseite, am Standort (Mitte) die östliche Bürgersteigseite. Zone 2 betrifft die Mitte der Straße, Zone 3 die vorgenannten gegenüberliegenden Bürgersteigseiten.</t>
   </si>
+  <si>
+    <t>Bei den Zählwerten **vor dem 03.03.2022** (Testbetrieb)  können Inkonsistenzen vorkommen. Ab dem 03.03.2022 ist die Datenqualität in der Regel gut.
+- Bei den Zählungen vor dem 03.03.2022 können Inkonsistenzen auftreten. Im Gebiet «Bahnhofstrasse (Süd)» stimmt bis zum 03.03.2022 die Unterscheidung zwischen Erwachsenen und Kindern nicht. Alle Zählwerte wurden in diesem Zeitraum fäschlicherweise den Kindern zugeordnet.
+- Im Teilgebiet **Bahnhofstrasse (Nord)** fehlen die Messwerte zwischen:
+   - dem 14.09. – 23.12.2022 
+   - dem 03.03. – 21.09.2023 
+wegen Bauarbeiten.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1203,11 +1207,11 @@
   <cellStyles count="7">
     <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1"/>
-    <cellStyle name="Standard 3" xfId="2"/>
-    <cellStyle name="Standard 4" xfId="3"/>
-    <cellStyle name="Standard 5" xfId="4"/>
-    <cellStyle name="Standard 6" xfId="5"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Standard 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Standard 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Standard 5" xfId="4" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Standard 6" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1448,27 +1452,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="28.625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="66.875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="53.625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="8.625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="88.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="50.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.08203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="28.58203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="66.83203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="53.58203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="8.58203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="88.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="50.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="255.5" style="1" customWidth="1"/>
     <col min="9" max="16384" width="255.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1491,7 +1495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
@@ -1509,7 +1513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
@@ -1520,14 +1524,14 @@
         <v>9</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>14</v>
       </c>
@@ -1545,7 +1549,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
@@ -1561,7 +1565,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>22</v>
       </c>
@@ -1579,7 +1583,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>26</v>
       </c>
@@ -1597,7 +1601,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>29</v>
       </c>
@@ -1615,7 +1619,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>32</v>
       </c>
@@ -1633,7 +1637,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>35</v>
       </c>
@@ -1651,7 +1655,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>38</v>
       </c>
@@ -1669,7 +1673,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>41</v>
       </c>
@@ -1685,7 +1689,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>44</v>
       </c>
@@ -1703,7 +1707,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>48</v>
       </c>
@@ -1721,7 +1725,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>52</v>
       </c>
@@ -1739,7 +1743,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>55</v>
       </c>
@@ -1757,7 +1761,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
         <v>59</v>
       </c>
@@ -1775,14 +1779,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="3"/>
       <c r="C18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>63</v>
       </c>
@@ -1795,7 +1799,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
         <v>8</v>
       </c>
@@ -1805,7 +1809,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:6" ht="147.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="150" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>65</v>
       </c>
@@ -1813,10 +1817,10 @@
         <v>257</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>65</v>
       </c>
@@ -1827,18 +1831,18 @@
         <v>255</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="125" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>65</v>
       </c>
       <c r="B23" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C23" s="21" t="s">
         <v>261</v>
       </c>
-      <c r="C23" s="21" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>65</v>
       </c>
@@ -1849,7 +1853,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>65</v>
       </c>
@@ -1860,7 +1864,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="25" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>65</v>
       </c>
@@ -1871,7 +1875,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
@@ -1881,7 +1885,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>
       <c r="D28" s="1"/>
@@ -1890,19 +1894,19 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="1"/>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="1"/>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1910,7 +1914,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>72</v>
       </c>
@@ -1926,7 +1930,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" s="4" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
       <c r="B33" s="13" t="s">
         <v>75</v>
@@ -1942,7 +1946,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" s="4" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>79</v>
       </c>
@@ -1954,7 +1958,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" s="4" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>79</v>
       </c>
@@ -1966,7 +1970,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" s="4" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>79</v>
       </c>
@@ -1978,7 +1982,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" s="4" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>79</v>
       </c>
@@ -1990,7 +1994,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" s="4" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>79</v>
       </c>
@@ -2002,7 +2006,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" s="4" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>79</v>
       </c>
@@ -2014,7 +2018,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" s="4" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>79</v>
       </c>
@@ -2026,7 +2030,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" s="4" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>79</v>
       </c>
@@ -2038,7 +2042,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" s="4" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>79</v>
       </c>
@@ -2050,7 +2054,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" s="4" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>79</v>
       </c>
@@ -2066,7 +2070,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>79</v>
       </c>
@@ -2082,7 +2086,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
         <v>79</v>
       </c>
@@ -2095,7 +2099,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
         <v>79</v>
       </c>
@@ -2108,7 +2112,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
         <v>79</v>
       </c>
@@ -2121,7 +2125,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
         <v>79</v>
       </c>
@@ -2134,7 +2138,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>79</v>
       </c>
@@ -2147,7 +2151,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
         <v>79</v>
       </c>
@@ -2160,7 +2164,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
         <v>79</v>
       </c>
@@ -2173,7 +2177,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
         <v>79</v>
       </c>
@@ -2186,7 +2190,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>79</v>
       </c>
@@ -2199,7 +2203,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
         <v>79</v>
       </c>
@@ -2212,7 +2216,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
         <v>79</v>
       </c>
@@ -2225,7 +2229,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>79</v>
       </c>
@@ -2238,7 +2242,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
         <v>79</v>
       </c>
@@ -2254,7 +2258,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
         <v>79</v>
       </c>
@@ -2267,7 +2271,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
         <v>79</v>
       </c>
@@ -2280,7 +2284,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
         <v>79</v>
       </c>
@@ -2293,7 +2297,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
         <v>79</v>
       </c>
@@ -2306,7 +2310,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
         <v>79</v>
       </c>
@@ -2319,7 +2323,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
         <v>79</v>
       </c>
@@ -2332,7 +2336,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="11" t="s">
         <v>79</v>
       </c>
@@ -2345,7 +2349,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="11" t="s">
         <v>79</v>
       </c>
@@ -2358,7 +2362,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="11" t="s">
         <v>79</v>
       </c>
@@ -2371,7 +2375,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="11" t="s">
         <v>79</v>
       </c>
@@ -2384,7 +2388,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
         <v>79</v>
       </c>
@@ -2397,7 +2401,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="11" t="s">
         <v>79</v>
       </c>
@@ -2413,7 +2417,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="11" t="s">
         <v>79</v>
       </c>
@@ -2426,7 +2430,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
         <v>79</v>
       </c>
@@ -2439,38 +2443,38 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="11"/>
       <c r="B72" s="21"/>
       <c r="C72" s="21"/>
       <c r="D72" s="21"/>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B73" s="21"/>
       <c r="C73" s="21"/>
       <c r="D73" s="21"/>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="7"/>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="7"/>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B77" s="3" t="s">
         <v>83</v>
       </c>
@@ -2478,13 +2482,13 @@
       <c r="D77" s="7"/>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="11" t="s">
         <v>84</v>
       </c>
@@ -2498,7 +2502,7 @@
       <c r="E79" s="6"/>
       <c r="F79" s="4"/>
     </row>
-    <row r="80" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" ht="25" x14ac:dyDescent="0.3">
       <c r="B80" s="13" t="s">
         <v>86</v>
       </c>
@@ -2511,7 +2515,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="11" t="s">
         <v>88</v>
       </c>
@@ -2521,7 +2525,7 @@
       <c r="E81" s="7"/>
       <c r="F81" s="7"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="11" t="s">
         <v>88</v>
       </c>
@@ -2531,7 +2535,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="7"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B83" s="12"/>
       <c r="C83" s="12"/>
       <c r="D83" s="12"/>
@@ -2545,146 +2549,146 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.375" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.125" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.625" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.875" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.625" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.375" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.375" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.875" style="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.625" style="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.375" style="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.625" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.625" style="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.875" style="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.08203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.58203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.58203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.08203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.58203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.58203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.58203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" style="24" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" style="24" customWidth="1"/>
     <col min="16" max="16384" width="11" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="31" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="32" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A24" r:id="rId1" location="metadata"/>
+    <hyperlink ref="A24" r:id="rId1" location="metadata" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.27559055118110237"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2692,22 +2696,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.5" style="24" customWidth="1"/>
-    <col min="2" max="2" width="5.625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="5.58203125" style="24" customWidth="1"/>
     <col min="3" max="3" width="11" style="24" customWidth="1"/>
     <col min="4" max="16384" width="11" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>89</v>
       </c>
@@ -2715,27 +2719,27 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>115</v>
       </c>
@@ -2743,19 +2747,19 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A11" r:id="rId1" location="metadata"/>
+    <hyperlink ref="A11" r:id="rId1" location="metadata" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.27559055118110237"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2763,22 +2767,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.375" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.125" style="24" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.08203125" style="24" customWidth="1"/>
     <col min="3" max="3" width="11" style="24" customWidth="1"/>
     <col min="4" max="16384" width="11" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>89</v>
       </c>
@@ -2786,123 +2790,123 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="30" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="26"/>
     </row>
-    <row r="19" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="26"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="32" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="26"/>
     </row>
-    <row r="23" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="26"/>
     </row>
-    <row r="24" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="26"/>
     </row>
-    <row r="25" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="26"/>
     </row>
-    <row r="26" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="26"/>
     </row>
-    <row r="27" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="26"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1" location="metadata"/>
+    <hyperlink ref="A21" r:id="rId1" location="metadata" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.27559055118110237"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2910,23 +2914,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.5" style="24" customWidth="1"/>
-    <col min="2" max="2" width="5.375" style="24" customWidth="1"/>
-    <col min="3" max="3" width="58.625" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="24" customWidth="1"/>
+    <col min="3" max="3" width="58.58203125" style="24" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="24" customWidth="1"/>
     <col min="5" max="16384" width="11" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>89</v>
       </c>
@@ -2937,7 +2941,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>133</v>
       </c>
@@ -2947,7 +2951,7 @@
       </c>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>135</v>
       </c>
@@ -2959,7 +2963,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>138</v>
       </c>
@@ -2971,7 +2975,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>141</v>
       </c>
@@ -2983,7 +2987,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>61</v>
       </c>
@@ -2995,7 +2999,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>146</v>
       </c>
@@ -3007,7 +3011,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
         <v>149</v>
       </c>
@@ -3019,7 +3023,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>152</v>
       </c>
@@ -3031,7 +3035,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>155</v>
       </c>
@@ -3041,7 +3045,7 @@
       </c>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>157</v>
       </c>
@@ -3051,7 +3055,7 @@
       </c>
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>159</v>
       </c>
@@ -3061,7 +3065,7 @@
       </c>
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>161</v>
       </c>
@@ -3073,7 +3077,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
         <v>164</v>
       </c>
@@ -3085,7 +3089,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>167</v>
       </c>
@@ -3095,7 +3099,7 @@
       </c>
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>169</v>
       </c>
@@ -3105,12 +3109,12 @@
       </c>
       <c r="D16"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="32" t="s">
         <v>110</v>
       </c>
@@ -3118,7 +3122,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A22" r:id="rId1" location="metadata"/>
+    <hyperlink ref="A22" r:id="rId1" location="metadata" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.27559055118110237"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Update for Prod and adding categories to metadata
</commit_message>
<xml_diff>
--- a/automation/hystreet_fussgaengerfrequenzen/hystreet_fussgaenger_metadata.xlsx
+++ b/automation/hystreet_fussgaengerfrequenzen/hystreet_fussgaenger_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszgua\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszgua\Python\git\opendatazurich.github.io\automation\hystreet_fussgaengerfrequenzen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F94B8D6-E116-4290-84D1-56B3AE0BAD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D15BAC-5639-4F03-9D5C-B8C37638208A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="-120" windowWidth="27855" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30060" yWindow="-7275" windowWidth="28110" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="283">
   <si>
     <t>Tagname</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Kategorie</t>
-  </si>
-  <si>
-    <t>Freizeit, Mobilität, Umwelt</t>
   </si>
   <si>
     <t>1-n Angaben aus den Werten des Sheets kategorien_werteliste.  z.B. Umwelt, Bevölkerung</t>
@@ -840,6 +837,69 @@
 Bei allen Gebieten und Zonen kann zwischen Erwachsenen und Kindern sowie nach der Laufrichtung (Bürkliplatz oder Hauptbahnhof) unterschieden werden. 
 Desweiteren beinhaltet der Datensatz auch Angaben zum Wetter und zur Temperatur während des Messzeitpunkts.</t>
   </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>arbeit-und-erwerb</t>
+  </si>
+  <si>
+    <t>basiskarten,</t>
+  </si>
+  <si>
+    <t>bauen-und-wohnen</t>
+  </si>
+  <si>
+    <t>bevolkerung</t>
+  </si>
+  <si>
+    <t>bildung</t>
+  </si>
+  <si>
+    <t>energie</t>
+  </si>
+  <si>
+    <t>finanzen</t>
+  </si>
+  <si>
+    <t>freizeit</t>
+  </si>
+  <si>
+    <t>gesundheit</t>
+  </si>
+  <si>
+    <t>kriminalitat</t>
+  </si>
+  <si>
+    <t>kultur</t>
+  </si>
+  <si>
+    <t>mobilitat</t>
+  </si>
+  <si>
+    <t>politik</t>
+  </si>
+  <si>
+    <t>preise</t>
+  </si>
+  <si>
+    <t>soziales</t>
+  </si>
+  <si>
+    <t>tourismus</t>
+  </si>
+  <si>
+    <t>umwelt</t>
+  </si>
+  <si>
+    <t>verwaltung</t>
+  </si>
+  <si>
+    <t>volkswirtschaft</t>
+  </si>
+  <si>
+    <t>freizeit, mobilitat, umwelt</t>
+  </si>
 </sst>
 </file>
 
@@ -848,13 +908,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1095,22 +1161,19 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1125,84 +1188,93 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="15" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="16" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1456,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1507,7 +1579,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
@@ -1525,7 +1597,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
@@ -1543,241 +1615,241 @@
         <v>9</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>16</v>
+        <v>282</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="C5" s="17" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>20</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="7"/>
       <c r="F5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>23</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>26</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>27</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>29</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>30</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>33</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>36</v>
-      </c>
       <c r="C10" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>39</v>
-      </c>
       <c r="C11" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>42</v>
-      </c>
       <c r="C12" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="9"/>
       <c r="F12" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>44</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>45</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>49</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="C16" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="20" t="s">
         <v>56</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>57</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>60</v>
-      </c>
       <c r="C17" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1789,13 +1861,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="C19" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -1805,75 +1877,75 @@
         <v>8</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="153" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>254</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B23" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="C23" s="21" t="s">
         <v>259</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="C24" s="21" t="s">
         <v>66</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
@@ -1883,7 +1955,7 @@
       <c r="D27" s="1"/>
       <c r="E27" s="7"/>
       <c r="F27" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1892,7 +1964,7 @@
       <c r="D28" s="1"/>
       <c r="E28" s="7"/>
       <c r="F28" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1917,10 +1989,10 @@
     </row>
     <row r="32" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>73</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>9</v>
@@ -1928,519 +2000,519 @@
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
       <c r="B33" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="D33" s="13" t="s">
         <v>76</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>77</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B34" s="21"/>
       <c r="C34" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B35" s="21"/>
       <c r="C35" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B36" s="21"/>
       <c r="C36" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B37" s="21"/>
       <c r="C37" s="21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B38" s="21"/>
       <c r="C38" s="21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B39" s="21"/>
       <c r="C39" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B40" s="21"/>
       <c r="C40" s="21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B41" s="21"/>
       <c r="C41" s="21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B42" s="21"/>
       <c r="C42" s="21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B43" s="21"/>
       <c r="C43" s="21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B44" s="21"/>
       <c r="C44" s="21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B45" s="21"/>
       <c r="C45" s="21" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B46" s="21"/>
       <c r="C46" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B47" s="21"/>
       <c r="C47" s="21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E47" s="7"/>
     </row>
     <row r="48" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B48" s="21"/>
       <c r="C48" s="21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B49" s="21"/>
       <c r="C49" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E49" s="7"/>
     </row>
     <row r="50" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B50" s="21"/>
       <c r="C50" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B51" s="21"/>
       <c r="C51" s="21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B52" s="21"/>
       <c r="C52" s="21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E52" s="7"/>
     </row>
     <row r="53" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B53" s="21"/>
       <c r="C53" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B54" s="21"/>
       <c r="C54" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B55" s="21"/>
       <c r="C55" s="21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B56" s="21"/>
       <c r="C56" s="21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D56" s="21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E56" s="7"/>
     </row>
     <row r="57" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B57" s="21"/>
       <c r="C57" s="21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E57" s="7"/>
       <c r="F57" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B58" s="21"/>
       <c r="C58" s="21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D58" s="21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E58" s="7"/>
     </row>
     <row r="59" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B59" s="21"/>
       <c r="C59" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E59" s="7"/>
     </row>
     <row r="60" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B60" s="21"/>
       <c r="C60" s="21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D60" s="21" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E60" s="7"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B61" s="21"/>
       <c r="C61" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D61" s="21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E61" s="7"/>
     </row>
     <row r="62" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B62" s="21"/>
       <c r="C62" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D62" s="21" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E62" s="7"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B63" s="21"/>
       <c r="C63" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D63" s="21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E63" s="7"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B64" s="21"/>
       <c r="C64" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D64" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E64" s="7"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B65" s="21"/>
       <c r="C65" s="21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D65" s="21" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E65" s="7"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B66" s="21"/>
       <c r="C66" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D66" s="21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E66" s="7"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B67" s="21"/>
       <c r="C67" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D67" s="21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E67" s="7"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B68" s="21"/>
       <c r="C68" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E68" s="7"/>
     </row>
     <row r="69" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B69" s="21"/>
       <c r="C69" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D69" s="21" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E69" s="7"/>
       <c r="F69" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="70" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B70" s="21"/>
       <c r="C70" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E70" s="7"/>
     </row>
     <row r="71" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B71" s="21"/>
       <c r="C71" s="21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E71" s="7"/>
     </row>
@@ -2477,7 +2549,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B77" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="7"/>
@@ -2491,13 +2563,13 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B79" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B79" s="9" t="s">
-        <v>85</v>
-      </c>
       <c r="C79" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="6"/>
@@ -2505,7 +2577,7 @@
     </row>
     <row r="80" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B80" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C80" s="13" t="s">
         <v>11</v>
@@ -2513,12 +2585,12 @@
       <c r="D80" s="13"/>
       <c r="E80" s="7"/>
       <c r="F80" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B81" s="12"/>
       <c r="C81" s="12"/>
@@ -2528,7 +2600,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B82" s="12"/>
       <c r="C82" s="12"/>
@@ -2551,10 +2623,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2577,114 +2649,174 @@
     <col min="16" max="16384" width="11" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="B2" s="35" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="B3" s="36" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
+      <c r="B4" s="36" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
+      <c r="B5" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
+      <c r="B6" s="35" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
+      <c r="B7" s="35" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
+      <c r="B8" s="35" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
+      <c r="B9" s="35" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="29" t="s">
+      <c r="B10" s="35" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="29" t="s">
+      <c r="B11" s="35" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
+      <c r="B12" s="35" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
+      <c r="B13" s="35" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="29" t="s">
+      <c r="B14" s="35" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="29" t="s">
+      <c r="B15" s="35" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
+      <c r="B16" s="35" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="29" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="29" t="s">
+      <c r="B17" s="35" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="29" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="29" t="s">
+      <c r="B18" s="35" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="29" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="29" t="s">
+      <c r="B19" s="35" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="29" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="29" t="s">
+      <c r="B20" s="35" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="31" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="32" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="32" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2714,48 +2846,48 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>115</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2785,90 +2917,90 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2879,12 +3011,12 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2933,191 +3065,191 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C1" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="28" t="s">
         <v>131</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D2"/>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" t="s">
         <v>136</v>
-      </c>
-      <c r="D3" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B4" s="26"/>
       <c r="C4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" t="s">
         <v>139</v>
-      </c>
-      <c r="D4" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5" s="26"/>
       <c r="C5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" t="s">
         <v>142</v>
-      </c>
-      <c r="D5" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" t="s">
         <v>144</v>
-      </c>
-      <c r="D6" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" t="s">
         <v>147</v>
-      </c>
-      <c r="D7" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" t="s">
         <v>150</v>
-      </c>
-      <c r="D8" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" t="s">
         <v>153</v>
-      </c>
-      <c r="D9" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D10"/>
     </row>
     <row r="11" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B11" s="26"/>
       <c r="C11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D11"/>
     </row>
     <row r="12" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B12" s="26"/>
       <c r="C12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D12"/>
     </row>
     <row r="13" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B13" s="26"/>
       <c r="C13" t="s">
+        <v>161</v>
+      </c>
+      <c r="D13" t="s">
         <v>162</v>
-      </c>
-      <c r="D13" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D14" t="s">
         <v>165</v>
-      </c>
-      <c r="D14" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D15"/>
     </row>
     <row r="16" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D16"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C22" s="26"/>
     </row>

</xml_diff>